<commit_message>
Dev hwj 1111 (#326)
* 成本信息表下载完成，总经理审批、营销部审批完成

* 问题清单720、722、723、724解决

* 成本信息数据问题修改

* 仅保存功能

* 仅保存功能开发

* 报价成本信息表问题处理

* 营销部审批，成本问题处理，报价反馈增加字段

* 报价反馈相关开发

* 报价出不来的问题解决

* 文件归档报价部分完成，报价看板问题处理

* 归档完成

* 梯度走量问题解决、738改变数据结构方便前端显示，756问题解决

* 客户目标价为0引发的成本问题解决，产品名改方案，梯度走量修改

* 因为汇率为空造成的异常问题解决

* 报价流程相关处理

* 报价分析看板无法显示问题处理

* 报价分析看板处理

* 审批表问题处理

* 保存优化

* 字段控制

* 增加报价方案删除接口，总经理审批二结构修改

---------

Co-authored-by: Zero656329 <hwj656329@163.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/新成本信息表模板.xlsx
+++ b/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/新成本信息表模板.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>密级：</t>
   </si>
@@ -357,6 +357,26 @@
   </si>
   <si>
     <t>{{PriceCost.QuSop}}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>方案名</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心组件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>型号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -789,7 +809,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,58 +973,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,11 +1021,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1072,7 +1095,7 @@
         <xdr:cNvPr id="2" name="Line 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1152,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018080000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1215,7 +1238,7 @@
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019080000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1301,7 +1324,7 @@
                   <a14:compatExt spid="_x0000_s3075"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A080000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1382,7 +1405,7 @@
         <xdr:cNvPr id="6" name="图片 5" descr="C:\Users\fbchen\AppData\Roaming\Foxmail7\Temp-6912-20210104080636\Attach\附件2-浙江舜宇智领技术有限公司logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,7 +1736,7 @@
   <dimension ref="B1:T38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M17" sqref="M16:M17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1780,24 +1803,24 @@
       <c r="I3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="70"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="2:19" ht="36" customHeight="1" thickBot="1">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
     </row>
     <row r="5" spans="2:19" ht="21" customHeight="1" thickTop="1">
       <c r="B5" s="51" t="s">
@@ -1867,11 +1890,11 @@
       <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
       <c r="F8" s="27"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -1911,20 +1934,20 @@
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
       <c r="F10" s="31"/>
       <c r="G10" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="33"/>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="58"/>
+      <c r="J10" s="61"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
       <c r="M10" s="31"/>
@@ -1959,20 +1982,20 @@
       <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="31"/>
       <c r="G12" s="25" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="31"/>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="69"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
@@ -1989,7 +2012,7 @@
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
-      <c r="G13" s="75" t="s">
+      <c r="G13" s="71" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="25"/>
@@ -2009,13 +2032,13 @@
       <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
       <c r="F14" s="31"/>
-      <c r="G14" s="76"/>
+      <c r="G14" s="72"/>
       <c r="H14" s="31"/>
       <c r="I14" s="26" t="s">
         <v>54</v>
@@ -2074,23 +2097,23 @@
       <c r="S16" s="7"/>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="67" t="s">
+      <c r="D17" s="66"/>
+      <c r="E17" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="63" t="s">
+      <c r="G17" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="73" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="31"/>
@@ -2106,13 +2129,13 @@
       <c r="S17" s="7"/>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="62"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="59"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="73"/>
       <c r="I18" s="25"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
@@ -2129,10 +2152,10 @@
       <c r="B19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="60"/>
+      <c r="D19" s="74"/>
       <c r="E19" s="22" t="s">
         <v>57</v>
       </c>
@@ -2179,9 +2202,9 @@
     </row>
     <row r="21" spans="2:20">
       <c r="B21" s="11"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="25"/>
@@ -2218,12 +2241,22 @@
       <c r="S22" s="7"/>
     </row>
     <row r="23" spans="2:20">
-      <c r="B23" s="4"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="E23" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="79" t="s">
+        <v>99</v>
+      </c>
       <c r="H23" s="25"/>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
@@ -2241,20 +2274,20 @@
       <c r="B24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="57"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="24" t="s">
         <v>62</v>
       </c>
       <c r="F24" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="57" t="s">
+      <c r="G24" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="57"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
@@ -2414,49 +2447,49 @@
       <c r="S29" s="7"/>
     </row>
     <row r="30" spans="2:20">
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="72" t="s">
+      <c r="C30" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="72" t="s">
+      <c r="D30" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72" t="s">
+      <c r="E30" s="76"/>
+      <c r="F30" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72" t="s">
+      <c r="G30" s="76"/>
+      <c r="H30" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72" t="s">
+      <c r="I30" s="76"/>
+      <c r="J30" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72" t="s">
+      <c r="K30" s="76"/>
+      <c r="L30" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72" t="s">
+      <c r="M30" s="76"/>
+      <c r="N30" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="O30" s="72"/>
-      <c r="P30" s="72" t="s">
+      <c r="O30" s="76"/>
+      <c r="P30" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="Q30" s="72"/>
-      <c r="R30" s="72" t="s">
+      <c r="Q30" s="76"/>
+      <c r="R30" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="S30" s="73"/>
+      <c r="S30" s="77"/>
       <c r="T30" s="29"/>
     </row>
     <row r="31" spans="2:20">
-      <c r="B31" s="74"/>
-      <c r="C31" s="72"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="76"/>
       <c r="D31" s="45" t="s">
         <v>41</v>
       </c>
@@ -2667,16 +2700,18 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:Q30"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="I12:J12"/>
@@ -2684,18 +2719,16 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>